<commit_message>
Peter picked QS domain
</commit_message>
<xml_diff>
--- a/PILOT_Status.xlsx
+++ b/PILOT_Status.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="50">
   <si>
     <t>ae.xpt</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>JJ</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reviewers Guide </t>
+  </si>
+  <si>
+    <t>references to DS and AE</t>
   </si>
 </sst>
 </file>
@@ -640,9 +649,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -978,19 +998,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="3" width="12.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="30">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1000,380 +1024,407 @@
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E4" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="E5" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="F10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D18" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
+      <c r="E23" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
+    <row r="30" spans="1:5">
+      <c r="A30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
+    <row r="31" spans="1:5">
+      <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
+    <row r="32" spans="1:5">
+      <c r="A32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" t="s">
+      <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
status as of 4-may-2017
</commit_message>
<xml_diff>
--- a/PILOT_Status.xlsx
+++ b/PILOT_Status.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
   <si>
     <t>ae.xpt</t>
   </si>
@@ -164,7 +164,13 @@
     <t xml:space="preserve"> Reviewers Guide </t>
   </si>
   <si>
-    <t>references to DS and AE</t>
+    <t>fix dataset name in xpt file</t>
+  </si>
+  <si>
+    <t>has references to DS and AE</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1007,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1024,6 +1030,9 @@
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="E1" s="2" t="s">
         <v>48</v>
       </c>
@@ -1081,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>26</v>
@@ -1098,11 +1107,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
@@ -1111,6 +1123,12 @@
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
@@ -1133,6 +1151,9 @@
       <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
@@ -1142,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1206,7 +1227,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>26</v>
@@ -1218,6 +1239,12 @@
       </c>
       <c r="B16" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:5">

</xml_diff>

<commit_message>
to do list as of 6/1
</commit_message>
<xml_diff>
--- a/PILOT_Status.xlsx
+++ b/PILOT_Status.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PeterS\Documents\CDISC_PhUSE\TestData\UpdatedPILOT02\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="315" windowWidth="16995" windowHeight="7710"/>
+    <workbookView xWindow="5436" yWindow="312" windowWidth="16992" windowHeight="7716"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
   <si>
     <t>ae.xpt</t>
   </si>
@@ -149,9 +154,6 @@
     <t>at14-0-02.sas</t>
   </si>
   <si>
-    <t>Nancy</t>
-  </si>
-  <si>
     <t>Jessica</t>
   </si>
   <si>
@@ -161,23 +163,23 @@
     <t>yes</t>
   </si>
   <si>
-    <t xml:space="preserve"> Reviewers Guide </t>
-  </si>
-  <si>
-    <t>fix dataset name in xpt file</t>
-  </si>
-  <si>
     <t>has references to DS and AE</t>
   </si>
   <si>
     <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Nancy/JJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReadMe Guide </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,7 +316,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,6 +494,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -655,18 +663,27 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -716,6 +733,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -762,7 +787,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -794,9 +819,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -828,6 +871,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1003,24 +1064,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="3" width="12.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="19" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="3" width="12.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1031,427 +1092,460 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="E1" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="3" t="s">
+      <c r="E23" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1462,12 +1556,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated after 06/15 meeting
</commit_message>
<xml_diff>
--- a/PILOT_Status.xlsx
+++ b/PILOT_Status.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,18 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5436" yWindow="312" windowWidth="16992" windowHeight="7716"/>
+    <workbookView xWindow="8580" yWindow="315" windowWidth="16995" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">files!$A$1:$F$36</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
   <si>
     <t>ae.xpt</t>
   </si>
@@ -163,16 +166,22 @@
     <t>yes</t>
   </si>
   <si>
-    <t>has references to DS and AE</t>
-  </si>
-  <si>
     <t>Assigned To</t>
   </si>
   <si>
-    <t>Nancy/JJ</t>
-  </si>
-  <si>
     <t xml:space="preserve">ReadMe Guide </t>
+  </si>
+  <si>
+    <t>split dataset because of size</t>
+  </si>
+  <si>
+    <t>pick up from Nancy</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>after AE completion, has references to DS and AE</t>
   </si>
 </sst>
 </file>
@@ -663,16 +672,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -681,10 +687,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1065,23 +1068,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="3" width="12.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="3" width="12.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="19" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="2"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1092,32 +1096,37 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1126,15 +1135,15 @@
       <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1143,15 +1152,15 @@
       <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1160,15 +1169,15 @@
       <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1177,30 +1186,35 @@
       <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1209,15 +1223,15 @@
       <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1226,27 +1240,38 @@
       <c r="D9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1255,13 +1280,13 @@
       <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1270,30 +1295,35 @@
       <c r="D12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1302,13 +1332,13 @@
       <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1317,28 +1347,33 @@
       <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1347,15 +1382,15 @@
       <c r="D17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1364,13 +1399,13 @@
       <c r="D18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1379,13 +1414,13 @@
       <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1394,9 +1429,9 @@
       <c r="D20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1409,11 +1444,11 @@
       <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1426,9 +1461,9 @@
       <c r="D22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1441,11 +1476,11 @@
       <c r="D23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
@@ -1453,7 +1488,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1461,7 +1496,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>41</v>
       </c>
@@ -1469,7 +1504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
@@ -1477,7 +1512,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
@@ -1485,7 +1520,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -1493,7 +1528,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
@@ -1501,7 +1536,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
@@ -1509,7 +1544,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
@@ -1517,7 +1552,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -1525,7 +1560,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
@@ -1533,7 +1568,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
@@ -1541,7 +1576,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1550,6 +1585,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F36">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="SDTM"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1561,7 +1603,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
plan for define.xml updates
</commit_message>
<xml_diff>
--- a/PILOT_Status.xlsx
+++ b/PILOT_Status.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="315" windowWidth="16995" windowHeight="7710"/>
+    <workbookView xWindow="13305" yWindow="315" windowWidth="16995" windowHeight="7710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">files!$A$1:$F$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">files!$A$1:$I$37</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="56">
   <si>
     <t>ae.xpt</t>
   </si>
@@ -172,22 +172,31 @@
     <t xml:space="preserve">ReadMe Guide </t>
   </si>
   <si>
-    <t>split dataset because of size</t>
-  </si>
-  <si>
-    <t>pick up from Nancy</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>after AE completion, has references to DS and AE</t>
+    <t>define.xml</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Update define.xml?</t>
+  </si>
+  <si>
+    <t>need to check after all updates</t>
+  </si>
+  <si>
+    <t>describe split dataset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -512,7 +521,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -627,6 +636,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -672,22 +690,28 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1067,42 +1091,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="3" width="12.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="11.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1110,23 +1149,23 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1135,15 +1174,18 @@
       <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1152,15 +1194,18 @@
       <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1169,15 +1214,18 @@
       <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1186,11 +1234,14 @@
       <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
@@ -1198,108 +1249,122 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -1307,49 +1372,53 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>51</v>
+      <c r="E13" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1357,23 +1426,26 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1382,15 +1454,18 @@
       <c r="D17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1399,13 +1474,15 @@
       <c r="D18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1414,13 +1491,15 @@
       <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1429,9 +1508,11 @@
       <c r="D20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1444,11 +1525,14 @@
       <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1461,9 +1545,11 @@
       <c r="D22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1476,129 +1562,140 @@
       <c r="D23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F36">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="SDTM"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I37" xr:uid="{C6E98F28-5FCE-4501-9FDA-AC051CB7EB6E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>